<commit_message>
Fix age in sessions.tsv for AIBL to BIDS clinical data converter
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications.xlsx
+++ b/clinica/iotools/data/clinical_specifications.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simona.bottani/clinica/clinica/iotools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorge.samper/ownCloud/Workspace/github/clinica/clinica/iotools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE756CCB-234A-E54E-BEEF-AF53AFC836C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="460" windowWidth="34020" windowHeight="19900" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="460" windowWidth="34020" windowHeight="19900" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
     <sheet name="sessions.tsv" sheetId="2" r:id="rId2"/>
     <sheet name="scans.tsv" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="939">
   <si>
     <t>Field</t>
   </si>
@@ -2874,7 +2875,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3183,6 +3184,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3204,7 +3208,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1025" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="1025" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3255,7 +3265,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3306,7 +3322,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3357,7 +3379,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3408,7 +3436,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3459,7 +3493,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3510,7 +3550,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3561,7 +3607,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3612,7 +3664,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3663,7 +3721,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3714,7 +3778,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3765,7 +3835,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3816,7 +3892,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3867,7 +3949,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3918,7 +4006,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3969,7 +4063,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4020,7 +4120,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4071,7 +4177,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4122,7 +4234,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4173,7 +4291,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="20" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4224,7 +4348,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="21" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4275,7 +4405,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="22" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4326,7 +4462,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="23" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4377,7 +4519,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="24" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4428,7 +4576,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="25" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4479,7 +4633,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="26" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4530,7 +4690,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="27" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4581,7 +4747,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvPr id="28" name="Rectangle 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4632,7 +4804,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="AutoShape 1"/>
+        <xdr:cNvPr id="29" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4688,7 +4866,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="AutoShape 1"/>
+        <xdr:cNvPr id="30" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4744,7 +4928,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="AutoShape 1"/>
+        <xdr:cNvPr id="31" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4800,7 +4990,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1024" name="AutoShape 1"/>
+        <xdr:cNvPr id="1024" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000000040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4856,7 +5052,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="AutoShape 1"/>
+        <xdr:cNvPr id="1026" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4912,7 +5114,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1027" name="AutoShape 1"/>
+        <xdr:cNvPr id="1027" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4968,7 +5176,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="AutoShape 1"/>
+        <xdr:cNvPr id="1028" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5024,7 +5238,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1029" name="AutoShape 1"/>
+        <xdr:cNvPr id="1029" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5080,7 +5300,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="AutoShape 1"/>
+        <xdr:cNvPr id="1030" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5136,7 +5362,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1031" name="AutoShape 1"/>
+        <xdr:cNvPr id="1031" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5192,7 +5424,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1032" name="AutoShape 1"/>
+        <xdr:cNvPr id="1032" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5248,7 +5486,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1033" name="AutoShape 1"/>
+        <xdr:cNvPr id="1033" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5304,7 +5548,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="AutoShape 1"/>
+        <xdr:cNvPr id="32" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5360,7 +5610,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="AutoShape 1"/>
+        <xdr:cNvPr id="33" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5416,7 +5672,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="AutoShape 1"/>
+        <xdr:cNvPr id="34" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5472,7 +5734,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="AutoShape 1"/>
+        <xdr:cNvPr id="35" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5528,7 +5796,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="AutoShape 1"/>
+        <xdr:cNvPr id="36" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5584,7 +5858,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="AutoShape 1"/>
+        <xdr:cNvPr id="37" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5640,7 +5920,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="AutoShape 1"/>
+        <xdr:cNvPr id="38" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5696,7 +5982,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="AutoShape 1"/>
+        <xdr:cNvPr id="39" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5752,7 +6044,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="AutoShape 1"/>
+        <xdr:cNvPr id="40" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5808,7 +6106,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="AutoShape 1"/>
+        <xdr:cNvPr id="41" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5864,7 +6168,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="AutoShape 1"/>
+        <xdr:cNvPr id="42" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5920,7 +6230,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="AutoShape 1"/>
+        <xdr:cNvPr id="43" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5976,7 +6292,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="AutoShape 1"/>
+        <xdr:cNvPr id="44" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6032,7 +6354,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name="AutoShape 1"/>
+        <xdr:cNvPr id="45" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6088,7 +6416,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="AutoShape 1"/>
+        <xdr:cNvPr id="46" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6126,6 +6460,114 @@
           <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13246100" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04FC6F13-9AD9-7342-B03F-FDF51A665098}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13982700" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -6394,11 +6836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6408,7 +6850,7 @@
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="28.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="77.33203125" style="1" customWidth="1"/>
@@ -15879,12 +16321,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N431"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15896,7 +16338,7 @@
     <col min="5" max="5" width="21" style="9" customWidth="1"/>
     <col min="6" max="6" width="65.6640625" style="9" customWidth="1"/>
     <col min="7" max="7" width="36" style="9" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="17.83203125" style="9" customWidth="1"/>
     <col min="12" max="12" width="21.5" style="9" customWidth="1"/>
@@ -15943,7 +16385,7 @@
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -15957,7 +16399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -15983,7 +16425,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -15992,6 +16434,12 @@
       </c>
       <c r="D4" s="9" t="s">
         <v>76</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>901</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>905</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16053,12 +16501,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>857</v>
       </c>
@@ -16071,10 +16519,10 @@
       <c r="G13" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="9" t="s">
         <v>906</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="9" t="s">
         <v>907</v>
       </c>
       <c r="J13" s="9" t="s">
@@ -20422,7 +20870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Bugfix and improve documentation (#181)
* Avoid bug with non string concatenation

* Fix missing fields in participants.tsv tab

* Clean scans.tsv tabs

* Add information to scan-level TSV files

* Add precision on ADNI downloading

* Transform errors in warning when image is missing in conversion_info
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications.xlsx
+++ b/clinica/iotools/data/clinical_specifications.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elina.thibeausutre/Documents/code/clinica/clinica/iotools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD2179-B2E3-A14D-92C1-EDDFF24ADDC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="1700" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1540" yWindow="1700" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
     <sheet name="sessions.tsv" sheetId="2" r:id="rId2"/>
     <sheet name="scans.tsv" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="955">
   <si>
     <t>Field</t>
   </si>
@@ -2904,12 +2905,33 @@
   </si>
   <si>
     <t>aibl_flutemeta_*.csv</t>
+  </si>
+  <si>
+    <t>CAPP</t>
+  </si>
+  <si>
+    <t>CAPP location</t>
+  </si>
+  <si>
+    <t>PREVDEMALS</t>
+  </si>
+  <si>
+    <t>PREVDEMALS location</t>
+  </si>
+  <si>
+    <t>Date IRM à M0</t>
+  </si>
+  <si>
+    <t>2016.07.04_CAPP_Database/M0</t>
+  </si>
+  <si>
+    <t>Date TEP à M0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3161,7 +3183,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3189,6 +3211,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="61">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -3286,7 +3311,7 @@
         <xdr:cNvPr id="1025" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3343,7 +3368,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3400,7 +3425,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3457,7 +3482,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3514,7 +3539,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3571,7 +3596,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3628,7 +3653,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3685,7 +3710,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3742,7 +3767,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3799,7 +3824,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3856,7 +3881,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3913,7 +3938,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3970,7 +3995,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4027,7 +4052,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4084,7 +4109,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4141,7 +4166,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4198,7 +4223,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4255,7 +4280,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4312,7 +4337,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4369,7 +4394,7 @@
         <xdr:cNvPr id="20" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4426,7 +4451,7 @@
         <xdr:cNvPr id="21" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4483,7 +4508,7 @@
         <xdr:cNvPr id="22" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4540,7 +4565,7 @@
         <xdr:cNvPr id="23" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4597,7 +4622,7 @@
         <xdr:cNvPr id="24" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4654,7 +4679,7 @@
         <xdr:cNvPr id="25" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4711,7 +4736,7 @@
         <xdr:cNvPr id="26" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4768,7 +4793,7 @@
         <xdr:cNvPr id="27" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4825,7 +4850,7 @@
         <xdr:cNvPr id="28" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4882,7 +4907,7 @@
         <xdr:cNvPr id="29" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4944,7 +4969,7 @@
         <xdr:cNvPr id="30" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5006,7 +5031,7 @@
         <xdr:cNvPr id="31" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5068,7 +5093,7 @@
         <xdr:cNvPr id="1024" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000000040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000000040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5130,7 +5155,7 @@
         <xdr:cNvPr id="1026" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5192,7 +5217,7 @@
         <xdr:cNvPr id="1027" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5254,7 +5279,7 @@
         <xdr:cNvPr id="1028" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5316,7 +5341,7 @@
         <xdr:cNvPr id="1029" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5378,7 +5403,7 @@
         <xdr:cNvPr id="1030" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5440,7 +5465,7 @@
         <xdr:cNvPr id="1031" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5502,7 +5527,7 @@
         <xdr:cNvPr id="1032" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5564,7 +5589,7 @@
         <xdr:cNvPr id="1033" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5626,7 +5651,7 @@
         <xdr:cNvPr id="32" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5688,7 +5713,7 @@
         <xdr:cNvPr id="33" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5750,7 +5775,7 @@
         <xdr:cNvPr id="34" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5812,7 +5837,7 @@
         <xdr:cNvPr id="35" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5874,7 +5899,7 @@
         <xdr:cNvPr id="36" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5936,7 +5961,7 @@
         <xdr:cNvPr id="37" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5998,7 +6023,7 @@
         <xdr:cNvPr id="38" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6060,7 +6085,7 @@
         <xdr:cNvPr id="39" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6122,7 +6147,7 @@
         <xdr:cNvPr id="40" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000028000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6184,7 +6209,7 @@
         <xdr:cNvPr id="41" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000029000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6246,7 +6271,7 @@
         <xdr:cNvPr id="42" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6308,7 +6333,7 @@
         <xdr:cNvPr id="43" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6370,7 +6395,7 @@
         <xdr:cNvPr id="44" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6432,7 +6457,7 @@
         <xdr:cNvPr id="45" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6494,7 +6519,7 @@
         <xdr:cNvPr id="46" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6556,7 +6581,7 @@
         <xdr:cNvPr id="47" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6610,7 +6635,7 @@
         <xdr:cNvPr id="48" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04FC6F13-9AD9-7342-B03F-FDF51A665098}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6664,7 +6689,7 @@
         <xdr:cNvPr id="49" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EA0262D6-9831-EA4A-95B3-7CDD3830145E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6715,7 +6740,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="AutoShape 1"/>
+        <xdr:cNvPr id="50" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6771,7 +6802,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="AutoShape 1"/>
+        <xdr:cNvPr id="51" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6827,7 +6864,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="AutoShape 1"/>
+        <xdr:cNvPr id="52" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6865,6 +6908,60 @@
           <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13982700" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -7133,7 +7230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH1021"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
@@ -16592,10 +16689,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N431"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G421" sqref="G421"/>
     </sheetView>
@@ -21141,238 +21238,303 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="3" width="23.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="21.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="2" max="3" width="14.5" style="27"/>
+    <col min="4" max="6" width="23.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="27" customWidth="1"/>
+    <col min="9" max="11" width="21.1640625" style="27" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>897</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>898</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>903</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>904</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="25" t="s">
+        <v>948</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>949</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>950</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>951</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>868</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>942</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="26" t="s">
+        <v>952</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>953</v>
+      </c>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>868</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>938</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="26" t="s">
+        <v>954</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>953</v>
+      </c>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>868</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>940</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>941</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>943</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>939</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>937</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="L7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>946</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>945</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F9" s="2" t="s">
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L9" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F10" s="2" t="s">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F11" s="2" t="s">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L11" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>868</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add loop diagnosis replacement for sessions, debug name-ses and xlsx
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications.xlsx
+++ b/clinica/iotools/data/clinical_specifications.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="942">
   <si>
     <t xml:space="preserve">Field</t>
   </si>
@@ -3269,9 +3269,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3281,7 +3281,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="25039440" cy="13092840"/>
+          <a:ext cx="25039800" cy="13092480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3314,9 +3314,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3326,7 +3326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="25039440" cy="13067640"/>
+          <a:ext cx="25039800" cy="13067280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3359,9 +3359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29160</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3371,7 +3371,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="25039440" cy="13448520"/>
+          <a:ext cx="25039800" cy="13448160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3404,9 +3404,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29160</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3416,7 +3416,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="25039440" cy="13448520"/>
+          <a:ext cx="25039800" cy="13448160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3449,9 +3449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29160</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3461,7 +3461,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="25039440" cy="13448520"/>
+          <a:ext cx="25039800" cy="13448160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3494,9 +3494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29160</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3506,7 +3506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="25039440" cy="13448520"/>
+          <a:ext cx="25039800" cy="13448160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3539,9 +3539,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29160</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3551,7 +3551,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="25039440" cy="13448520"/>
+          <a:ext cx="25039800" cy="13448160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3584,9 +3584,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>592560</xdr:colOff>
+      <xdr:colOff>592200</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3596,7 +3596,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="20074680" cy="13054680"/>
+          <a:ext cx="20075040" cy="13054320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3629,9 +3629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
+      <xdr:colOff>722160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3641,7 +3641,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="24709320" cy="13054680"/>
+          <a:ext cx="24709680" cy="13054320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3674,9 +3674,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
+      <xdr:colOff>722160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3686,7 +3686,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="24709320" cy="13054680"/>
+          <a:ext cx="24709680" cy="13054320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3719,9 +3719,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
+      <xdr:colOff>722160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3731,7 +3731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="24709320" cy="13054680"/>
+          <a:ext cx="24709680" cy="13054320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3764,9 +3764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
+      <xdr:colOff>722160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3776,7 +3776,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="24709320" cy="13054680"/>
+          <a:ext cx="24709680" cy="13054320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3809,9 +3809,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3821,7 +3821,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13270680"/>
+          <a:ext cx="13585320" cy="13270320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3854,9 +3854,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3866,7 +3866,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3899,9 +3899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3911,7 +3911,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3944,9 +3944,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3956,7 +3956,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3989,9 +3989,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4001,7 +4001,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4034,9 +4034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4046,7 +4046,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4079,9 +4079,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4091,7 +4091,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4124,9 +4124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4136,7 +4136,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4169,9 +4169,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4181,7 +4181,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4214,9 +4214,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4226,7 +4226,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4259,9 +4259,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4271,7 +4271,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4304,9 +4304,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1497960</xdr:colOff>
+      <xdr:colOff>1497600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4316,7 +4316,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13584960" cy="13080240"/>
+          <a:ext cx="13585320" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4349,9 +4349,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>926280</xdr:colOff>
+      <xdr:colOff>925920</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4361,7 +4361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10015560" cy="13080240"/>
+          <a:ext cx="10015920" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4394,9 +4394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>926280</xdr:colOff>
+      <xdr:colOff>925920</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4406,7 +4406,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10015560" cy="13080240"/>
+          <a:ext cx="10015920" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4439,9 +4439,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>926280</xdr:colOff>
+      <xdr:colOff>925920</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4451,7 +4451,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10015560" cy="13080240"/>
+          <a:ext cx="10015920" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4484,9 +4484,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>926280</xdr:colOff>
+      <xdr:colOff>925920</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4496,7 +4496,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10015560" cy="13080240"/>
+          <a:ext cx="10015920" cy="13079880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4530,7 +4530,7 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -5350,7 +5350,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M9" activeCellId="0" sqref="M9"/>
+      <selection pane="topRight" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5619,8 +5619,14 @@
       <c r="J20" s="11" t="s">
         <v>58</v>
       </c>
+      <c r="K20" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L20" s="11" t="s">
         <v>58</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9910,7 +9916,7 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adapt form bids compliance
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications.xlsx
+++ b/clinica/iotools/data/clinical_specifications.xlsx
@@ -9914,10 +9914,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10052,6 +10052,8 @@
         <v>933</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>